<commit_message>
Debugging, but haven't fixed averages yet. Their's a problem involving how weight is summed.
</commit_message>
<xml_diff>
--- a/Surveys/Response MatrixM777.xlsx
+++ b/Surveys/Response MatrixM777.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="145">
   <si>
     <t>1a</t>
   </si>
@@ -300,15 +300,9 @@
     <t>m777</t>
   </si>
   <si>
-    <t>Characteristic</t>
-  </si>
-  <si>
     <t>Stakeholder</t>
   </si>
   <si>
-    <t>Score</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -319,6 +313,153 @@
   </si>
   <si>
     <t>ii</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>CharacteristicNumber</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>iii</t>
+  </si>
+  <si>
+    <t>iv</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>vi</t>
   </si>
 </sst>
 </file>
@@ -519,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -578,7 +719,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -867,13 +1007,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G155"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="H136" sqref="H136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="18.7109375" style="1"/>
+    <col min="1" max="16384" width="18.7109375" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -881,15 +1021,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="21"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
     </row>
@@ -972,10 +1112,10 @@
         <v>8</v>
       </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="22"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
     </row>
@@ -1051,15 +1191,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="22"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="3"/>
       <c r="F24" s="4"/>
     </row>
@@ -1085,8 +1225,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="12"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="10"/>
@@ -1140,10 +1279,10 @@
         <v>12</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="22"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="3"/>
       <c r="F36" s="4"/>
     </row>
@@ -1224,10 +1363,10 @@
         <v>20</v>
       </c>
       <c r="B47" s="3"/>
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="22"/>
+      <c r="D47" s="21"/>
       <c r="E47" s="3"/>
       <c r="F47" s="4"/>
     </row>
@@ -1309,10 +1448,10 @@
         <v>28</v>
       </c>
       <c r="B58" s="3"/>
-      <c r="C58" s="21" t="s">
+      <c r="C58" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D58" s="22"/>
+      <c r="D58" s="21"/>
       <c r="E58" s="3"/>
       <c r="F58" s="4"/>
     </row>
@@ -1391,10 +1530,10 @@
         <v>30</v>
       </c>
       <c r="B70" s="3"/>
-      <c r="C70" s="21" t="s">
+      <c r="C70" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D70" s="22"/>
+      <c r="D70" s="21"/>
       <c r="E70" s="3"/>
       <c r="F70" s="4"/>
     </row>
@@ -1474,10 +1613,10 @@
         <v>38</v>
       </c>
       <c r="B81" s="3"/>
-      <c r="C81" s="21" t="s">
+      <c r="C81" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D81" s="22"/>
+      <c r="D81" s="21"/>
       <c r="E81" s="3"/>
       <c r="F81" s="4"/>
     </row>
@@ -1557,10 +1696,10 @@
         <v>46</v>
       </c>
       <c r="B93" s="3"/>
-      <c r="C93" s="21" t="s">
+      <c r="C93" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D93" s="22"/>
+      <c r="D93" s="21"/>
       <c r="E93" s="3"/>
       <c r="F93" s="4"/>
     </row>
@@ -1640,10 +1779,10 @@
         <v>54</v>
       </c>
       <c r="B105" s="3"/>
-      <c r="C105" s="21" t="s">
+      <c r="C105" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="D105" s="22"/>
+      <c r="D105" s="21"/>
       <c r="E105" s="3"/>
       <c r="F105" s="4"/>
     </row>
@@ -1722,10 +1861,10 @@
         <v>61</v>
       </c>
       <c r="B117" s="3"/>
-      <c r="C117" s="21" t="s">
+      <c r="C117" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D117" s="22"/>
+      <c r="D117" s="21"/>
       <c r="E117" s="3"/>
       <c r="F117" s="4"/>
     </row>
@@ -1804,10 +1943,10 @@
         <v>69</v>
       </c>
       <c r="B129" s="3"/>
-      <c r="C129" s="21" t="s">
+      <c r="C129" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="D129" s="22"/>
+      <c r="D129" s="21"/>
       <c r="E129" s="3"/>
       <c r="F129" s="4"/>
     </row>
@@ -1833,7 +1972,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
-      <c r="D131" s="9"/>
+      <c r="B131" s="9"/>
       <c r="E131" s="13"/>
       <c r="F131" s="10"/>
     </row>
@@ -1887,10 +2026,10 @@
         <v>77</v>
       </c>
       <c r="B141" s="3"/>
-      <c r="C141" s="21" t="s">
+      <c r="C141" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D141" s="22"/>
+      <c r="D141" s="21"/>
       <c r="E141" s="3"/>
       <c r="F141" s="4"/>
     </row>
@@ -1915,8 +2054,8 @@
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" s="9"/>
-      <c r="C143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="13"/>
       <c r="D143" s="18"/>
       <c r="E143" s="18"/>
       <c r="F143" s="10"/>
@@ -1924,9 +2063,8 @@
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="11"/>
       <c r="B144" s="12"/>
-      <c r="C144" s="13"/>
       <c r="D144" s="12"/>
-      <c r="E144" s="12"/>
+      <c r="E144" s="9"/>
       <c r="F144" s="14"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -1967,7 +2105,9 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="9"/>
+      <c r="A152" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="B152" s="1" t="s">
         <v>86</v>
       </c>
@@ -1989,6 +2129,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="C141:D141"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C81:D81"/>
@@ -1996,12 +2142,6 @@
     <mergeCell ref="C105:D105"/>
     <mergeCell ref="C117:D117"/>
     <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C47:D47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2010,852 +2150,951 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16:E17"/>
+      <selection activeCell="A2" sqref="A2:XFD130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
         <v>92</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
         <v>95</v>
       </c>
-      <c r="D1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="I4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5">
+        <v>0.5</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>144</v>
+      </c>
+      <c r="F11">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+      <c r="F12">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>119</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
         <v>30</v>
       </c>
-      <c r="B3">
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>140</v>
+      </c>
+      <c r="F18">
         <v>1</v>
       </c>
-      <c r="D3">
+      <c r="G18">
         <v>5</v>
       </c>
-      <c r="E3">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="G19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="B4">
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F21">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="E4">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="G22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
         <v>46</v>
       </c>
-      <c r="B5">
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="G24">
         <v>5</v>
       </c>
-      <c r="E5">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
+      <c r="G25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26">
         <v>1</v>
       </c>
-      <c r="D6">
+      <c r="G26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>140</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31">
+        <v>0.5</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32">
+        <v>0.5</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
         <v>2</v>
       </c>
-      <c r="E6">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" t="s">
+        <v>95</v>
+      </c>
+      <c r="F33">
+        <v>0.5</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="H34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
+        <v>102</v>
+      </c>
+      <c r="E36" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15">
+      <c r="G36">
         <v>4</v>
       </c>
-      <c r="E15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17">
-        <v>4</v>
-      </c>
-      <c r="E17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>3</v>
-      </c>
-      <c r="E19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
-        <v>2</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="D22">
-        <v>4</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="D23">
+      <c r="H36">
         <v>5</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>5</v>
-      </c>
-      <c r="E24">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-      <c r="E25">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-      <c r="E27">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-      <c r="E28">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>3</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>5</v>
-      </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="D32">
-        <v>3</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="D33">
-        <v>5</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="D34">
-        <v>3</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="20">
-        <v>2</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>3</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="D38">
-        <v>6</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
-      </c>
-      <c r="E39">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="D40">
-        <v>5</v>
-      </c>
-      <c r="E40">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="D41">
-        <v>6</v>
-      </c>
-      <c r="E41">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="D42">
-        <v>3</v>
-      </c>
-      <c r="E42">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="D43">
-        <v>4</v>
-      </c>
-      <c r="E43">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="D44">
-        <v>5</v>
-      </c>
-      <c r="E44">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="D45">
-        <v>3</v>
-      </c>
-      <c r="E45">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="D46">
-        <v>5</v>
-      </c>
-      <c r="E46">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="D47">
-        <v>6</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48">
-        <v>3</v>
-      </c>
-      <c r="D48">
-        <v>3</v>
-      </c>
-      <c r="E48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B49">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>96</v>
-      </c>
-      <c r="D49">
-        <v>4</v>
-      </c>
-      <c r="E49">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>97</v>
-      </c>
-      <c r="D50">
-        <v>5</v>
-      </c>
-      <c r="E50">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-      <c r="D51">
-        <v>4</v>
-      </c>
-      <c r="E51">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
-        <v>97</v>
-      </c>
-      <c r="D52">
-        <v>4</v>
-      </c>
-      <c r="E52">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
-      <c r="C53" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53">
-        <v>4</v>
-      </c>
-      <c r="E53">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B54">
-        <v>3</v>
-      </c>
-      <c r="C54" t="s">
-        <v>97</v>
-      </c>
-      <c r="D54">
-        <v>4</v>
-      </c>
-      <c r="E54">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55">
-        <v>3</v>
-      </c>
-      <c r="C55" t="s">
-        <v>96</v>
-      </c>
-      <c r="D55">
-        <v>4</v>
-      </c>
-      <c r="E55">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B56">
-        <v>3</v>
-      </c>
-      <c r="C56" t="s">
-        <v>97</v>
-      </c>
-      <c r="D56">
-        <v>5</v>
-      </c>
-      <c r="E56">
-        <v>0.5</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G54">
-    <sortCondition ref="B2:B54"/>
-    <sortCondition ref="A2:A54"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>